<commit_message>
docs(metrics): update dashboard with real test data, 79.6% pass rate and 10 real bugs
</commit_message>
<xml_diff>
--- a/Test Metrics/Test_Metrics_Dashboard.xlsx
+++ b/Test Metrics/Test_Metrics_Dashboard.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\hockyVII\kiem_thu_phan_mem\bai_tap\MANUAL-TESTING-GROUP-3\Test Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E42006-A3F4-4583-8CDB-9EE27B5B8360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1435EDB1-1BCA-43E8-A72C-E846386A588B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F9DC949F-D471-4B0D-8B80-731C764C9F65}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Metrics" sheetId="2" r:id="rId2"/>
+    <sheet name="Metrics" sheetId="6" r:id="rId2"/>
     <sheet name="Chart" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>STT</t>
   </si>
@@ -58,18 +58,6 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Bug Critical</t>
-  </si>
-  <si>
-    <t>Bug Major</t>
-  </si>
-  <si>
-    <t>Bug Minor</t>
-  </si>
-  <si>
-    <t>Authentication</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -79,34 +67,88 @@
     <t>Checkout</t>
   </si>
   <si>
-    <t>General (Footer)</t>
-  </si>
-  <si>
     <t>SUM</t>
   </si>
   <si>
     <t>TỔNG CỘNG</t>
   </si>
   <si>
-    <t>1. Tỷ lệ thực thi (Test Execution Rate)</t>
-  </si>
-  <si>
-    <t>2. Tỷ lệ Đạt/Hỏng (Pass/Fail Rate)</t>
-  </si>
-  <si>
-    <t>4. Phân bố mức độ nghiêm trọng (Severity Distribution)</t>
-  </si>
-  <si>
-    <t>Công thức: (Tổng số TC đã chạy / Tổng số TC quy hoạch) * 100%</t>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Mức độ</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Số Bug</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>Phân hệ (Module)</t>
+  </si>
+  <si>
+    <t>Đạt (Pass)</t>
+  </si>
+  <si>
+    <t>Hỏng (Fail)</t>
+  </si>
+  <si>
+    <t>Lỗi Critical</t>
+  </si>
+  <si>
+    <t>Lỗi Major</t>
+  </si>
+  <si>
+    <t>Lỗi Minor</t>
+  </si>
+  <si>
+    <t>Tổng Lỗi</t>
+  </si>
+  <si>
+    <t>Xác thực (Auth)</t>
+  </si>
+  <si>
+    <t>Sản phẩm (Product)</t>
+  </si>
+  <si>
+    <t>Giỏ hàng (Cart)</t>
+  </si>
+  <si>
+    <t>Thanh toán (Checkout)</t>
+  </si>
+  <si>
+    <t>1. Tỷ lệ thực thi (Test Execution Rate):</t>
+  </si>
+  <si>
+    <t>2. Tỷ lệ Đạt/Hỏng (Pass/Fail Rate):</t>
+  </si>
+  <si>
+    <t>3. Mật độ lỗi theo Module (Defect Density):</t>
+  </si>
+  <si>
+    <t>4. Phân bố mức độ nghiêm trọng (Severity Distribution):</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Giá trị: </t>
+      <t xml:space="preserve">Chạy 54/54 TC $\rightarrow$ Đạt </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -115,51 +157,67 @@
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> (54/54)</t>
+      <t xml:space="preserve"> (Thỏa mãn Exit Criteria).</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Đánh giá:</t>
+      <t xml:space="preserve">Tỷ lệ Pass: (43 / 54) * 100 = </t>
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <b/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> Đạt yêu cầu Exit Criteria.</t>
+      <t>79.6%</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Pass Rate: (45 / 54) * 100% = </t>
+      <t xml:space="preserve">Tỷ lệ Fail: (11 / 54) * 100 = </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>83.3%</t>
+      <t>20.4%</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Fail Rate: (9 / 54) * 100% = </t>
+      <t xml:space="preserve">Xác thực (Auth): 3 Bugs / 15 TCs = </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>20.0%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sản phẩm (Product): 2 Bugs / 12 TCs = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -169,88 +227,42 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">3. Mật độ lỗi theo Module (Defect Density) - </t>
+      <t xml:space="preserve">Giỏ hàng (Cart): 3 Bugs / 15 TCs = </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <i/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Quan trọng</t>
+      <t>20.0%</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Auth: 3 Bugs / 15 TCs = </t>
+      <t xml:space="preserve">Thanh toán (Checkout): 2 Bugs / 12 TCs = </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>20%</t>
+      <t>16.7%</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Product: 2 Bugs / 12 TCs = </t>
+      <t>Nghiêm trọng (Critical): 3 Lỗi (</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>16.6%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cart: 2 Bugs / 15 TCs = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>13.3%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Checkout: 2 Bugs / 12 TCs = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>16.6%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Critical: 3 Bugs (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -259,7 +271,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -269,12 +281,12 @@
   </si>
   <si>
     <r>
-      <t>Major: 4 Bugs (</t>
+      <t>Lớn (Major): 4 Lỗi (</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -283,7 +295,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -293,12 +305,12 @@
   </si>
   <si>
     <r>
-      <t>Minor: 3 Bugs (</t>
+      <t>Nhỏ (Minor): 3 Lỗi (</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -307,7 +319,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
@@ -316,99 +328,64 @@
     </r>
   </si>
   <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
-    <t>Số lượng</t>
-  </si>
-  <si>
-    <t>Mức độ</t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>Minor</t>
-  </si>
-  <si>
-    <t>Số Bug</t>
-  </si>
-  <si>
-    <t>Auth</t>
-  </si>
-  <si>
-    <t>Footer</t>
-  </si>
-  <si>
-    <t>NHẬN XÉT CHẤT LƯỢNG (QUALITY ASSESSMENT):</t>
-  </si>
-  <si>
     <r>
-      <t>1. Mức độ rủi ro:</t>
+      <t>ĐÁNH GIÁ CHẤT LƯỢNG (QUALITY ASSESSMENT):</t>
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> CAO (High). Dự án đang tồn tại </t>
+      <t xml:space="preserve"> Dựa trên quá trình kiểm thử thực tế trên hệ thống, QA Team đưa ra kết luận:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Cảnh báo rủi ro (High Risk):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Tỷ lệ Pass Rate chỉ đạt </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>30% lỗi Critical</t>
+      <t>79.6%</t>
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> (3 lỗi nghiêm trọng) ảnh hưởng trực tiếp đến tính năng thanh toán và bảo mật.</t>
+      <t xml:space="preserve"> (Dưới mức kỳ vọng 90%). Hệ thống đang chứa 3 lỗi Critical cực kỳ nguy hiểm: Lỗ hổng XSS trên thanh tìm kiếm, cho phép nhập số lượng âm (-5) vào giỏ hàng, và Form thanh toán thẻ không hề có bước xác thực (Fake Payment validation).</t>
     </r>
   </si>
   <si>
     <r>
-      <t>2. Điểm nóng (Hotspot):</t>
+      <t>2. Phân bổ lỗi:</t>
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> Module </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Authentication</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> có mật độ lỗi cao nhất (20%) và chứa lỗ hổng bảo mật SQL Injection.</t>
+      <t xml:space="preserve"> Lỗi phân bổ rải rác ở tất cả các phân hệ, đặc biệt khu vực Giỏ hàng và Xác thực có mật độ lỗi cao nhất (20%).</t>
     </r>
   </si>
   <si>
@@ -417,12 +394,12 @@
     </r>
     <r>
       <rPr>
-        <sz val="13"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> Hệ thống chưa đạt tiêu chuẩn để Release. Cần khắc phục toàn bộ 3 lỗi Critical và 4 lỗi Major, sau đó thực hiện kiểm thử hồi quy (Regression Test).</t>
+      <t xml:space="preserve"> Mã nguồn (Source Code) hiện tại được code khá sơ sài, thiếu Validation ở Backend. Kiến nghị KHÔNG RELEASE phiên bản này. Cần đưa code về trạng thái Fix Bug khẩn cấp.</t>
     </r>
   </si>
 </sst>
@@ -430,7 +407,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,43 +417,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="13"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="13"/>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -501,40 +471,288 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF1F1F1F"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -546,7 +764,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -565,7 +783,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -584,7 +802,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -603,7 +821,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -622,7 +840,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -641,7 +859,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -660,7 +878,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -679,7 +897,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -698,7 +916,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -717,7 +935,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
@@ -736,241 +954,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13"/>
+        <sz val="12"/>
         <color rgb="FF1F1F1F"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color rgb="FF1F1F1F"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1191,10 +1181,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1461,9 +1451,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$20:$A$24</c:f>
+              <c:f>Data!$A$20:$A$23</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Auth</c:v>
                 </c:pt>
@@ -1476,18 +1466,15 @@
                 <c:pt idx="3">
                   <c:v>Checkout</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>Footer</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$20:$B$24</c:f>
+              <c:f>Data!$B$20:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1495,13 +1482,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3807,53 +3791,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18128A0C-89A6-45B4-A9D0-23F86628579C}" name="Table1" displayName="Table1" ref="A1:I7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:I7" xr:uid="{18128A0C-89A6-45B4-A9D0-23F86628579C}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{119E43FE-CDE5-4585-8716-B8BEBB5B8B3C}" name="STT" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{10B687D3-900C-451F-A7D7-632C36041D71}" name="Module" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{776ACBBB-EF3E-4E53-9C2A-524EDE8DAF1B}" name="Tổng số TC" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{34C19E27-F7CF-460A-B2B0-EC2DA110DFD5}" name="Đã chạy (Executed)" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{73D3B2B5-6C67-4AB2-8B76-EF3F05FA16E3}" name="Pass" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{FE13216E-8300-4681-A84B-EB090D546FEC}" name="Fail" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{D1D32F2A-4B3F-41C5-BB86-4DBE56E01269}" name="Bug Critical" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{07EFF4F3-7171-4FF2-8304-94C74DA2F736}" name="Bug Major" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{34F3CBBC-F3E1-4DD4-8E99-3C8001AFAEEF}" name="Bug Minor" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8855C291-4BD7-4007-93B6-52D2214EA40A}" name="Table2" displayName="Table2" ref="A10:B12" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A10:B12" xr:uid="{8855C291-4BD7-4007-93B6-52D2214EA40A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C0540476-BA7A-402D-AB27-B1FBDB64686C}" name="Trạng thái" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{79B142FE-AAE5-4F64-9BD8-BFFCC6DFAF03}" name="Số lượng" dataDxfId="22"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8855C291-4BD7-4007-93B6-52D2214EA40A}" name="Table2" displayName="Table2" ref="A10:B12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
-  <autoFilter ref="A10:B12" xr:uid="{8855C291-4BD7-4007-93B6-52D2214EA40A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{594863F1-00F7-4E7C-BD93-C9974500F113}" name="Table3" displayName="Table3" ref="A14:B17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A14:B17" xr:uid="{594863F1-00F7-4E7C-BD93-C9974500F113}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C0540476-BA7A-402D-AB27-B1FBDB64686C}" name="Trạng thái" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{79B142FE-AAE5-4F64-9BD8-BFFCC6DFAF03}" name="Số lượng" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{0693D044-E618-4028-8CBE-C165D2E7D3F3}" name="Mức độ" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{C16E7A7E-791A-4853-9C57-01CA788BE733}" name="Số lượng" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{594863F1-00F7-4E7C-BD93-C9974500F113}" name="Table3" displayName="Table3" ref="A14:B17" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
-  <autoFilter ref="A14:B17" xr:uid="{594863F1-00F7-4E7C-BD93-C9974500F113}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C3176B89-DE43-47B8-8AE8-E10E0BD1B86F}" name="Table5" displayName="Table5" ref="A19:B23" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A19:B23" xr:uid="{C3176B89-DE43-47B8-8AE8-E10E0BD1B86F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0693D044-E618-4028-8CBE-C165D2E7D3F3}" name="Mức độ" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{C16E7A7E-791A-4853-9C57-01CA788BE733}" name="Số lượng" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{FBC9CC3B-9B71-4257-BD75-E46EC5C1A56D}" name="Module" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{85054B3E-8EE2-4946-9FA3-A9129EBDE163}" name="Số Bug" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C3176B89-DE43-47B8-8AE8-E10E0BD1B86F}" name="Table5" displayName="Table5" ref="A19:B24" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A19:B24" xr:uid="{C3176B89-DE43-47B8-8AE8-E10E0BD1B86F}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FBC9CC3B-9B71-4257-BD75-E46EC5C1A56D}" name="Module" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{85054B3E-8EE2-4946-9FA3-A9129EBDE163}" name="Số Bug" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1C6E713B-069B-4468-9E27-38D962E37507}" name="Table49" displayName="Table49" ref="A1:J6" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:J6" xr:uid="{1C6E713B-069B-4468-9E27-38D962E37507}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{B9DFF633-261B-4A78-AA95-037DB3E536CC}" name="STT" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{5A7DE9B3-2668-4959-8648-F29CA9770F5F}" name="Phân hệ (Module)" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{6CC342AA-9A32-43EA-9D9E-9720B8BB687F}" name="Tổng số TC" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{6299E704-95EA-4F85-B40F-13EA3B86FC40}" name="Đã chạy (Executed)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{8C0D5233-5CAD-492E-A86F-D61B55114E28}" name="Đạt (Pass)" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{32DA6A9B-5A91-4530-9402-D03BFFBD5A6E}" name="Hỏng (Fail)" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{474C994A-AB63-40A6-A405-C688C2E7DFBA}" name="Lỗi Critical" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{234B544A-C240-4E16-BBEB-8E67E1EFE9D9}" name="Lỗi Major" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{4D396435-6B59-4EE2-94B8-2C263A468803}" name="Lỗi Minor" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{B4E33ABD-FA89-4937-AB95-094D082101B1}" name="Tổng Lỗi" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4174,351 +4159,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F487311-4717-46A7-A274-5304F43364EA}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.46484375" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" customWidth="1"/>
-    <col min="8" max="8" width="12.06640625" customWidth="1"/>
-    <col min="9" max="9" width="12.19921875" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="20.53125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="20.46484375" style="8" customWidth="1"/>
+    <col min="5" max="6" width="9.06640625" style="8"/>
+    <col min="7" max="7" width="13.3984375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="12.06640625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="12.19921875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>54</v>
+      </c>
+      <c r="D6" s="2">
+        <v>54</v>
+      </c>
+      <c r="E6" s="2">
+        <v>43</v>
+      </c>
+      <c r="F6" s="2">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="B12" s="11">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11">
+        <v>4</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="B21" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="B22" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A23" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.45">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4">
-        <v>15</v>
-      </c>
-      <c r="E2" s="4">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="4">
+      <c r="B23" s="11">
         <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4">
-        <v>2</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.45">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4">
-        <v>2</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="33" x14ac:dyDescent="0.45">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="33" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3">
-        <v>54</v>
-      </c>
-      <c r="D7" s="3">
-        <v>54</v>
-      </c>
-      <c r="E7" s="3">
-        <v>45</v>
-      </c>
-      <c r="F7" s="3">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3</v>
-      </c>
-      <c r="H7" s="3">
-        <v>4</v>
-      </c>
-      <c r="I7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2">
-        <v>45</v>
-      </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="2">
-        <v>9</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2">
-        <v>3</v>
-      </c>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="2">
-        <v>4</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:2" ht="33" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="33" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="33" x14ac:dyDescent="0.45">
-      <c r="A23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4534,132 +4513,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAE2E98-0D8B-46D3-B84B-E3E861A95AD4}">
-  <dimension ref="A1:A31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124EAF92-056B-4A54-A656-7B9BFCECA69B}">
+  <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="9.06640625" style="6"/>
+    <col min="1" max="16384" width="9.06640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
+      <c r="A1" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" s="7"/>
+      <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" s="7"/>
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" s="7" t="s">
-        <v>20</v>
+      <c r="A5" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A7" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" s="7"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" s="7" t="s">
-        <v>22</v>
+      <c r="A11" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" s="7"/>
+      <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="A13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" s="5"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" s="7"/>
+      <c r="A16" s="5"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="7" t="s">
-        <v>25</v>
+      <c r="A17" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="7"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" s="7"/>
+      <c r="A19" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" s="7" t="s">
-        <v>27</v>
+      <c r="A21" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" s="7"/>
+      <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="A23" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" s="5"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" s="7"/>
+      <c r="A26" s="5"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" s="7"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" s="7" t="s">
-        <v>31</v>
+      <c r="A27" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -4671,7 +4634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC09771-5E5A-4B7D-BF2F-8DF568DCE210}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="V24" sqref="I18:V24"/>
     </sheetView>
   </sheetViews>

</xml_diff>